<commit_message>
feat(ui): handle empty expense table state
</commit_message>
<xml_diff>
--- a/Brainstorm expenseTracker.xlsx
+++ b/Brainstorm expenseTracker.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YUVRAJ\Desktop\expenseTracker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YUVRAJ\Desktop\expenseTracker\Simple-Expense-Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F3A9C5D-4CCF-409E-A55D-D40331E92280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD817C4-7E52-413F-8E52-93EE5706A1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Backlog" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="73">
   <si>
     <t>TS</t>
   </si>
@@ -191,9 +190,6 @@
     <t>All expenses displayed in table</t>
   </si>
   <si>
-    <t>No expenses stored state</t>
-  </si>
-  <si>
     <t>“No expenses recorded yet” displayed in table body</t>
   </si>
   <si>
@@ -228,6 +224,27 @@
   </si>
   <si>
     <t>Data remains visible and unchanged</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>“No expenses recorded yet” displayed in table body when table is empty</t>
+  </si>
+  <si>
+    <t>No expenses stored state when there is no data</t>
+  </si>
+  <si>
+    <t>No expenses stored state when data is added</t>
+  </si>
+  <si>
+    <t>1) Clear LocalStorage 2) Reload app 3) Add some data</t>
+  </si>
+  <si>
+    <t>“No expenses recorded yet” should disappera and new data should be updated</t>
+  </si>
+  <si>
+    <t>“No expenses recorded yet” idsappears in table body and new data is displayed</t>
   </si>
 </sst>
 </file>
@@ -565,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -760,7 +777,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>51</v>
       </c>
@@ -777,132 +794,164 @@
         <v>18</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>37</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+        <v>71</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
+    <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
@@ -995,6 +1044,10 @@
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat(expense): add new expense with validation and persistence
</commit_message>
<xml_diff>
--- a/Brainstorm expenseTracker.xlsx
+++ b/Brainstorm expenseTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YUVRAJ\Desktop\expenseTracker\Simple-Expense-Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD817C4-7E52-413F-8E52-93EE5706A1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72BC737-7F74-4D58-BB34-520939CBEBDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="75">
   <si>
     <t>TS</t>
   </si>
@@ -245,6 +245,12 @@
   </si>
   <si>
     <t>“No expenses recorded yet” idsappears in table body and new data is displayed</t>
+  </si>
+  <si>
+    <t>All expenses are displayed in table</t>
+  </si>
+  <si>
+    <t>Validation message shown, "Please enter amount."</t>
   </si>
 </sst>
 </file>
@@ -585,7 +591,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -662,8 +668,12 @@
       <c r="H2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="3" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -688,10 +698,14 @@
         <v>33</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+        <v>74</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -721,7 +735,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -774,8 +788,12 @@
       <c r="H6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">

</xml_diff>

<commit_message>
feat(expense): delete expense from list
</commit_message>
<xml_diff>
--- a/Brainstorm expenseTracker.xlsx
+++ b/Brainstorm expenseTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YUVRAJ\Desktop\expenseTracker\Simple-Expense-Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72BC737-7F74-4D58-BB34-520939CBEBDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86313FB9-5B4B-4F70-9141-E2F6D0C4E7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="75">
   <si>
     <t>TS</t>
   </si>
@@ -590,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -732,8 +732,12 @@
       <c r="H4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -760,8 +764,12 @@
       <c r="H5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -859,7 +867,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>55</v>
       </c>
@@ -884,8 +892,12 @@
       <c r="H9" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="I9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">

</xml_diff>

<commit_message>
feat(summary): calculate current month expense total
</commit_message>
<xml_diff>
--- a/Brainstorm expenseTracker.xlsx
+++ b/Brainstorm expenseTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YUVRAJ\Desktop\expenseTracker\Simple-Expense-Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86313FB9-5B4B-4F70-9141-E2F6D0C4E7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977AC44D-4AEA-495A-BCDF-1AD34734E750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="75">
   <si>
     <t>TS</t>
   </si>
@@ -88,9 +88,6 @@
     <t>Delete an expense from list</t>
   </si>
   <si>
-    <t>Calculate monthly total</t>
-  </si>
-  <si>
     <t>Category-wise total calculation</t>
   </si>
   <si>
@@ -208,9 +205,6 @@
     <t>TS_04</t>
   </si>
   <si>
-    <t>Total equals sum of expenses for that month</t>
-  </si>
-  <si>
     <t>Category totals calculated correctly</t>
   </si>
   <si>
@@ -251,6 +245,12 @@
   </si>
   <si>
     <t>Validation message shown, "Please enter amount."</t>
+  </si>
+  <si>
+    <t>Total equals sum of expenses for current calender month</t>
+  </si>
+  <si>
+    <t>Calculate current monthly total</t>
   </si>
 </sst>
 </file>
@@ -591,7 +591,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -616,10 +616,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -628,7 +628,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>4</v>
@@ -648,13 +648,13 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>9</v>
@@ -663,16 +663,16 @@
         <v>10</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -680,13 +680,13 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>11</v>
@@ -695,16 +695,16 @@
         <v>12</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -712,13 +712,13 @@
         <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>11</v>
@@ -727,7 +727,7 @@
         <v>14</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>13</v>
@@ -736,7 +736,7 @@
         <v>13</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -744,13 +744,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>9</v>
@@ -759,30 +759,30 @@
         <v>15</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>9</v>
@@ -791,94 +791,94 @@
         <v>17</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="J8" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>9</v>
@@ -887,98 +887,102 @@
         <v>19</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+        <v>73</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="G12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -1099,7 +1103,7 @@
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="3"/>
     </row>
@@ -1109,7 +1113,7 @@
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="3"/>
     </row>
@@ -1119,7 +1123,7 @@
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="3"/>
     </row>
@@ -1129,7 +1133,7 @@
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="3"/>
     </row>
@@ -1139,7 +1143,7 @@
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="3"/>
     </row>
@@ -1149,7 +1153,7 @@
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="3"/>
     </row>
@@ -1159,7 +1163,7 @@
     </row>
     <row r="15" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="3"/>
     </row>

</xml_diff>

<commit_message>
feat(summary): calculate category-wise expense totals
</commit_message>
<xml_diff>
--- a/Brainstorm expenseTracker.xlsx
+++ b/Brainstorm expenseTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YUVRAJ\Desktop\expenseTracker\Simple-Expense-Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977AC44D-4AEA-495A-BCDF-1AD34734E750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BC455F-14EA-4D04-AEA6-25FFDCFE537F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="75">
   <si>
     <t>TS</t>
   </si>
@@ -590,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -956,8 +956,12 @@
       <c r="H11" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
+      <c r="I11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -984,8 +988,12 @@
       <c r="H12" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
+      <c r="I12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>

</xml_diff>